<commit_message>
Diccionario de la WBS V. 3.0
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/Diccionario de la WBS.xlsx
+++ b/Planificación del proyecto/Diccionario de la WBS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Desktop\New folder (2)\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,263 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziUA
-Damian Santos    (2020-09-06 11:50:18)
-Cambiar el nombre de la carpeta a Proyectos de Software - Grupo 01.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziUE
-Damian Santos    (2020-09-06 11:50:43)
-Armar una carpeta que se llame Alcance. Dentro de esa, una que se llame versión 1. Y ahí poner los archivos de WBS.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTE
-Damian Santos    (2020-09-06 11:33:45)
-Por qué no están las vistas para el checkout? Están en el propio 1.5? Por qué algunas las separan y otras no?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziS4
-Damian Santos    (2020-09-06 11:30:32)
-Cómo medirían esto?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziS8
-Damian Santos    (2020-09-06 11:31:36)
-Son las vistas o el proceso? Eso no está en el 1.3.3?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTA
-Damian Santos    (2020-09-06 11:32:52)
-Cuáles son? No se podía agregar directamente al 1.6?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTI
-Damian Santos    (2020-09-06 11:35:45)
-Dónde gestiono lo que va en el slider y los artículos promocionados?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTo
-Damian Santos    (2020-09-06 11:45:37)
-El nombre no tiene relación con la descripción del entregable. Filtros y ordenamientos deberían estar aparte o ponerle un nombre más general al entregable</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTU
-Damian Santos    (2020-09-06 11:41:07)
-Esto se buscaba en el home, no como parte del catálogo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTs
-Damian Santos    (2020-09-06 11:46:16)
-Esto no debería estar dentro del catálogo? o de la vista de cada producto?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTw
-Damian Santos    (2020-09-06 11:46:56)
-Lo principal no es que ingrese los datos sino que confirme la compra (ingresando datos...)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B35" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTQ
-Damian Santos    (2020-09-06 11:37:56)
-Los ABMs no son de backoffice?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B36" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziTM
-Damian Santos    (2020-09-06 11:36:48)
-El nombre no me dice que se cargan artículos. Sería mejor algo del estilo: Importación de Artículos en Excel</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C39" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziT0
-Damian Santos    (2020-09-06 11:48:09)
-Acá hay mucho para decir y hacer. Incluso hasta se pueden disparar otros abms. Redefinir.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C43" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziT4
-Damian Santos    (2020-09-06 11:48:33)
-No existe un ABM de carritos. Para qué lo necesitaría?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B45" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>======
-ID#AAAAJ5YziT8
-Damian Santos    (2020-09-06 11:49:45)
-Cómo acceden los usuarios al backoffice?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miOz8j5sbAqDo5ennpjA9QTVzEpKw=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="268">
   <si>
     <t>Esta es una versión simplificada para el diccionario de la WBS.</t>
   </si>
@@ -368,9 +113,6 @@
     <t>Interfaz visual comprensible para el acceso o el registro al sistema</t>
   </si>
   <si>
-    <t>Que el registro solicite la cantidad necesaria de datos y permita el rápido acceso al sistema</t>
-  </si>
-  <si>
     <t>1.1.2</t>
   </si>
   <si>
@@ -396,9 +138,6 @@
   </si>
   <si>
     <t>Proceso de visualizacion de un slider principal, una sección con productos destacados y un menú con opciones para ir a la página con información institucional, al catálogo completo de productos y a un formulario de contacto.</t>
-  </si>
-  <si>
-    <t>Interfaz del home principal</t>
   </si>
   <si>
     <t>Debe tener un slider con promociones y una sección con productos destacados. Además, tendrá un menú con
@@ -407,9 +146,6 @@
   </si>
   <si>
     <t>Que ubique en el lugar adecuado las diferentes opciones, que no esté sobrecargado de información, que muestre un aspecto profesional</t>
-  </si>
-  <si>
-    <t>1.2</t>
   </si>
   <si>
     <t>Back Office</t>
@@ -474,18 +210,12 @@
     <t>Que tenga la compatibilidad necesaria para ser publicado en FaceBook</t>
   </si>
   <si>
-    <t>1.3</t>
-  </si>
-  <si>
     <t>Servicios al usuario</t>
   </si>
   <si>
     <t>Procesos de asignación de capacidades para el cliente</t>
   </si>
   <si>
-    <t xml:space="preserve">Que el cliente sea capaz de llevar a cabo </t>
-  </si>
-  <si>
     <t>Que el usuario se sienta cómo usando las distintas funciones, las cuales le permitirán gestionar sus pedidos y comprar de un modo sencillo</t>
   </si>
   <si>
@@ -519,9 +249,6 @@
     <t>Que sea personalizable, que se pueda ver de la forma que uno guste, que permita filtros con el fin de encontrar lo que se busca más rápidamente</t>
   </si>
   <si>
-    <t>1.3.2.1</t>
-  </si>
-  <si>
     <t>Proceso con el fin de permitir al usuario buscar por palabras, analizando los textos para el nombre y las descripciones, filtrar por categorías y subcategorías, ordenar por mayor precio, menor precio, nombre ascendente, nombre descendente.</t>
   </si>
   <si>
@@ -534,9 +261,6 @@
     <t>Que otorgue una correcta separación de productos para evitar ver contenido no buscado</t>
   </si>
   <si>
-    <t>1.3.2.2</t>
-  </si>
-  <si>
     <t>Productos destacados</t>
   </si>
   <si>
@@ -547,9 +271,6 @@
   </si>
   <si>
     <t>Que se le recomiende al cliente productos de calidad y utilidad basado en opiniones y compras</t>
-  </si>
-  <si>
-    <t>1.3.2.3</t>
   </si>
   <si>
     <t>Productos relacionados</t>
@@ -595,9 +316,6 @@
     <t>Que se le brinde ayuda ante las dudas o problemas que le surjan</t>
   </si>
   <si>
-    <t>1.3.5</t>
-  </si>
-  <si>
     <t>Descuentos personalizados</t>
   </si>
   <si>
@@ -611,9 +329,6 @@
   </si>
   <si>
     <t>Que se premie a aquellos clientes que son activos o que compran periódicamente</t>
-  </si>
-  <si>
-    <t>1.3.6</t>
   </si>
   <si>
     <t>Comentarios y calificaciones</t>
@@ -629,9 +344,6 @@
     <t>Que se sepa qué opinan los clientes sobre ciertos productos para que el resta sepa lo que realmente comprarán</t>
   </si>
   <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t>Checkout</t>
   </si>
   <si>
@@ -642,9 +354,6 @@
   </si>
   <si>
     <t>Que permita resguardar los datos asociados al pago y al destino de entrega, junto con una correcta administracion de los mismos, proporcionando seguridad al usuario</t>
-  </si>
-  <si>
-    <t>1.5.1</t>
   </si>
   <si>
     <t>Pagos</t>
@@ -663,9 +372,6 @@
     <t>Que sea seguro y confiable</t>
   </si>
   <si>
-    <t>1.5.2</t>
-  </si>
-  <si>
     <t>Envio</t>
   </si>
   <si>
@@ -679,9 +385,6 @@
   </si>
   <si>
     <t>Que los servicios otorgados le sean cómodos al cliente, mostrando las distintas alternativas posibles</t>
-  </si>
-  <si>
-    <t>1.6</t>
   </si>
   <si>
     <t>ABMs</t>
@@ -700,9 +403,6 @@
     <t>Correcta validacion de cada una de las operaciónes principales a cada uno de los componentes con el fin de garantizar el procesamiento adecuado de los datos y el mantenimiento de los mismos</t>
   </si>
   <si>
-    <t>1.6.1</t>
-  </si>
-  <si>
     <t>ABM de Producto</t>
   </si>
   <si>
@@ -718,9 +418,6 @@
     <t>Correcta validacion de cada una de las operaciónes principales asociadas a los productos con el fin de garantizar el procesamiento adecuado de sus propiedades y el mantenimiento de los mismos</t>
   </si>
   <si>
-    <t>1.6.2</t>
-  </si>
-  <si>
     <t>ABM Carrito</t>
   </si>
   <si>
@@ -736,27 +433,6 @@
     <t>Correcta validacion de cada una de las operaciónes principales asociadas a los carritos con el fin de garantizar el procesamiento adecuado de sus propiedades y el mantenimiento de los mismos</t>
   </si>
   <si>
-    <t>1.6.3</t>
-  </si>
-  <si>
-    <t>ABM Catalogo</t>
-  </si>
-  <si>
-    <t>Proceso de alta baja y modificación de la entidad catálogo</t>
-  </si>
-  <si>
-    <t>Alta, Baja y Modificación del catálogo de productos</t>
-  </si>
-  <si>
-    <t>Capacidad de alta baja y modificación del catago</t>
-  </si>
-  <si>
-    <t>Correcta validacion de cada una de las operaciónes principales asociadas al catalogo con el fin de garantizar el procesamiento adecuado de sus propiedades y el mantenimiento de los mismos</t>
-  </si>
-  <si>
-    <t>1.6.4</t>
-  </si>
-  <si>
     <t>ABM Usuario</t>
   </si>
   <si>
@@ -772,9 +448,6 @@
     <t>Correcta validacion de cada una de las operaciónes principales orientadas a los usuarios con el fin de garantizar el procesamiento adecuado de sus propiedades y el mantenimiento de los mismos</t>
   </si>
   <si>
-    <t>1.6.5</t>
-  </si>
-  <si>
     <t>ABM Pedido</t>
   </si>
   <si>
@@ -790,9 +463,6 @@
     <t>Correcta validacion de cada una de las operaciónes principales orientadas a los pedidos con el fin de garantizar el procesamiento adecuado de sus propiedades y el mantenimiento de los mismos</t>
   </si>
   <si>
-    <t>1.7</t>
-  </si>
-  <si>
     <t>Administración del proyecto</t>
   </si>
   <si>
@@ -808,9 +478,6 @@
     <t>Que se cumpla la planificacion respetando los tiempos y pudiendo entregar calidad al cliente según los requerimientos</t>
   </si>
   <si>
-    <t>1.7.1</t>
-  </si>
-  <si>
     <t>Inicio</t>
   </si>
   <si>
@@ -826,9 +493,6 @@
     <t>Que la WBS sea clara sobre la vision a futuro con respecto al proyecto</t>
   </si>
   <si>
-    <t>1.7.2</t>
-  </si>
-  <si>
     <t>Planificacion</t>
   </si>
   <si>
@@ -844,9 +508,6 @@
     <t>Que se cumplan los tiempos de planificacion y prevenir errores,  perdidas revisando y evaluando cada etapa</t>
   </si>
   <si>
-    <t>1.7.3</t>
-  </si>
-  <si>
     <t>Ejecucion</t>
   </si>
   <si>
@@ -862,9 +523,6 @@
     <t>Controlar los elementos de manera acorde para que no surjan imprevistos.</t>
   </si>
   <si>
-    <t>1.7.4</t>
-  </si>
-  <si>
     <t>Monitoreo y Control</t>
   </si>
   <si>
@@ -880,9 +538,6 @@
     <t>Comprobar que no haya errores  testeando todos los casos de uso posibles</t>
   </si>
   <si>
-    <t>1.7.5</t>
-  </si>
-  <si>
     <t>Cierre</t>
   </si>
   <si>
@@ -913,15 +568,6 @@
     <t>Video</t>
   </si>
   <si>
-    <t xml:space="preserve">Proceso con el fin de generar un codigo denominado SKU unico a partir de la combinacion de atributos que elija el cliente. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proceso para añadir imágenes descriptivas a un producto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proceso para añadir video a un producto </t>
-  </si>
-  <si>
     <t>Organización del catalogo</t>
   </si>
   <si>
@@ -971,13 +617,284 @@
   </si>
   <si>
     <t>Exportador de productos a formato facebook</t>
+  </si>
+  <si>
+    <t>Proceso por el cual se desarrollara un  slider donde se publicaran
+promociones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proceso por el cual se desarrollara una sección con productos destacados con el fin de facilitar la venta</t>
+  </si>
+  <si>
+    <t>Proceso por el cual se agregarán imágenes (cargándolas directamente o ingresando una URL)</t>
+  </si>
+  <si>
+    <t>Proceso con el fin de brindar al usuario su informacion dentro del e-commerce y donde ademas sera capaz de editarla</t>
+  </si>
+  <si>
+    <t>Proceso con el fin de gestionar la modificación de la contraseña de usuario</t>
+  </si>
+  <si>
+    <t>Proceso mediante el cual el usuario podra recuperar la contraseña a partir del mail del usuario</t>
+  </si>
+  <si>
+    <t>Proceso que tiene la finalidad de enviar un mensaje al vendedor en caso de que se confirme el pedido</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceso por el cual se asignará un código de referencia a los artículos para poder identificarlos de acuerdo a sus preferencias, por ejemplo colores y talle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>s.</t>
+    </r>
+  </si>
+  <si>
+    <t>Proceso por el cual de adjuntarán videos (desde una URL) del producto presentado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceso por el cual se asociará cada categoría a una de las opciones de la taxonomía de Google de acuerdo a características en común.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceso por el cual se gestionarán todas las funcionalidades de los usuarios para ingresar al sistema y mantener sus datos resguardados, así como también la configuración de sus preferencias tales como su perfil.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Home principal</t>
+  </si>
+  <si>
+    <t>Imagen</t>
+  </si>
+  <si>
+    <t>Proceso por el cual se permitirá la entrada (inputs) de datos para ingresar el domicilio y el método de pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceso en donde mediante dos campos, mail (de usuario) e información (mensaje) el usuario podra aclarar sus dudas o soporte que requiera 
+</t>
+  </si>
+  <si>
+    <t>Gestion del home</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>1.1.6</t>
+  </si>
+  <si>
+    <t>1.1.6.1</t>
+  </si>
+  <si>
+    <t>1.1.6.2</t>
+  </si>
+  <si>
+    <t>1.2.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.3</t>
+  </si>
+  <si>
+    <t>1.2.1.4</t>
+  </si>
+  <si>
+    <t>1.2.1.5</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>1.2.3.1</t>
+  </si>
+  <si>
+    <t>1.2.3.2</t>
+  </si>
+  <si>
+    <t>1.2.3.3</t>
+  </si>
+  <si>
+    <t>1.2.3.4</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>1.2.5</t>
+  </si>
+  <si>
+    <t>1.2.6</t>
+  </si>
+  <si>
+    <t>1.2.7</t>
+  </si>
+  <si>
+    <t>1.2.7.1</t>
+  </si>
+  <si>
+    <t>1.2.7.2</t>
+  </si>
+  <si>
+    <t>1.2.7.3</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>1.3.3.1</t>
+  </si>
+  <si>
+    <t>1.3.3.2</t>
+  </si>
+  <si>
+    <t>1.3.3.3</t>
+  </si>
+  <si>
+    <t>1.3.3.1.1</t>
+  </si>
+  <si>
+    <t>1.3.3.1.2</t>
+  </si>
+  <si>
+    <t>1.3.3.1.3</t>
+  </si>
+  <si>
+    <t>1.3.3.4</t>
+  </si>
+  <si>
+    <t>Proceso por el cual se gestionará lo que va en el slider y los artículos promocionados</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>1.4.2</t>
+  </si>
+  <si>
+    <t>1.4.3</t>
+  </si>
+  <si>
+    <t>1.4.4</t>
+  </si>
+  <si>
+    <t>1.4.5</t>
+  </si>
+  <si>
+    <t>Deslizador de imágenes con el fin de mostrar al cliente las promociones</t>
+  </si>
+  <si>
+    <t>Todas las funciones asociadas/orientadas al usuario</t>
+  </si>
+  <si>
+    <t>Que al vendedor se le mande un mensaje con la confirmacion del pedido</t>
+  </si>
+  <si>
+    <t>Que el codigo sea unico y que se genere en base a los atributos del producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que permita renderizar la imagen para una correcta visualización </t>
+  </si>
+  <si>
+    <t>Que permita la correcta visualizacion del video descriptivo acerca del producto</t>
+  </si>
+  <si>
+    <t>Que el mesaje de confirmación llegue en tiempo y forma al vendedor</t>
+  </si>
+  <si>
+    <t>A cada producto asignará un código de referencia para poder identificarlos de acuerdo a sus propiedades</t>
+  </si>
+  <si>
+    <t>Asociar imágenes a los distintos productos para agregar una descripcion visual de los mismos</t>
+  </si>
+  <si>
+    <t>Asociar un video a los distintos productos para agregar una descripcion visual de los mismos</t>
+  </si>
+  <si>
+    <t>Proceso por el cual se presenta la documentación sobre la planificación estratégica del e-commerce</t>
+  </si>
+  <si>
+    <t>Que la recuperacion de la clave sea segura con el proposito de resguardar los datos del usuario, y se lleve a cabo de la manera más pronta posible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el cambio de clave sea de forma segura, y que se realicen las validaciones necesarias para cumplir dicho objetivo. </t>
+  </si>
+  <si>
+    <t>Que el registro solicite la cantidad necesaria de datos y permita el rápido acceso al sistema. Brindando ayuda en todo momento para mejorar la experiencia</t>
+  </si>
+  <si>
+    <t>Permitir a los "usuarios" nuevos de la pagina la capacidad de registrarse con el fin de poder realizar las transacciones con mayor facilidad</t>
+  </si>
+  <si>
+    <t>Realizar comprobaciones de seguridad asociadas, cumpliendo que el registro sea unico por persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceso por el cual se guardarán los datos de un nuevo usuario </t>
+  </si>
+  <si>
+    <t>Permitir al usuario la correcta administracion de los distintos componentes del sitio, permitiendo que sea lo mas intuitiva para el usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacidad de administrar los elementos del home a traves de las vistas de las vistas </t>
+  </si>
+  <si>
+    <t>Presentar al usuario la informacion asociada a la cuenta, con la posibilidad de cambiar los datos de la misma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que la gestion de las disitintas cuentas sea lo más segura posible asegurando el resguardo de datos , y además que no presente inconvenientes al gestor </t>
+  </si>
+  <si>
+    <t>Interfaz visual intuitiva con el fin de que el usuario pueda consultar sus dudas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Que la interfaz permita que el usuario pueda consultar sus dudas y estas sean respondidas en el menor tiempo posible</t>
+  </si>
+  <si>
+    <t>Que los productos sean asociados adecuadamente según su categoria, para que google pueda recomendar dichos productos</t>
+  </si>
+  <si>
+    <t>Interfaz visual intuitiva para la carga de datos asociados con los medios de pago y el envio de los productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relacionará cada categoría una de las opciones de la taxonomía de Google de acuerdo a características en común.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1025,8 +942,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1035,8 +969,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBE5F1"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFDBE5F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFDBE5F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1108,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1123,41 +1075,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1166,26 +1085,125 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1213,9 +1231,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Diccionario-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1233,12 +1251,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A3:G11">
   <tableColumns count="7">
     <tableColumn id="1" name="ID "/>
-    <tableColumn id="2" name="Nombre "/>
-    <tableColumn id="3" name="Descripción "/>
-    <tableColumn id="4" name="Responsable "/>
-    <tableColumn id="5" name="Entregables "/>
-    <tableColumn id="6" name="Requisitos"/>
-    <tableColumn id="7" name="Calidad"/>
+    <tableColumn id="2" name="Nombre " dataDxfId="5"/>
+    <tableColumn id="3" name="Descripción " dataDxfId="4"/>
+    <tableColumn id="4" name="Responsable " dataDxfId="3"/>
+    <tableColumn id="5" name="Entregables " dataDxfId="2"/>
+    <tableColumn id="6" name="Requisitos" dataDxfId="1"/>
+    <tableColumn id="7" name="Calidad" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Diccionario-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1441,21 +1459,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.375" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
     <col min="2" max="2" width="22.875" customWidth="1"/>
     <col min="3" max="3" width="56.875" customWidth="1"/>
     <col min="4" max="4" width="27.25" customWidth="1"/>
     <col min="5" max="5" width="31.25" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="6" max="6" width="29.5" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
     <col min="8" max="18" width="9.375" customWidth="1"/>
     <col min="19" max="19" width="28.875" customWidth="1"/>
@@ -1494,1001 +1512,1160 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="11">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="25" t="s">
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="25" t="s">
+      <c r="B13" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="25" t="s">
+      <c r="B14" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="23"/>
-    </row>
-    <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="25" t="s">
+      <c r="B17" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="B18" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E18" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="E19" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="E20" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="36">
+        <v>1.3</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="C35" s="12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="D35" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="B36" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="E36" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="B37" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="E37" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="E38" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="E39" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="E40" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="B46" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="E46" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="E47" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="8" t="s">
+      <c r="E48" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="E49" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="E50" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="6"/>
+    </row>
+    <row r="51" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" s="8" t="s">
+      <c r="E51" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="G51" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
+      <c r="Y51" s="8"/>
+      <c r="Z51" s="8"/>
+    </row>
+    <row r="52" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="10" t="s">
+      <c r="E52" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F52" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G52" s="16" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="16"/>
-      <c r="N50" s="16"/>
-      <c r="O50" s="16"/>
-      <c r="P50" s="16"/>
-      <c r="Q50" s="16"/>
-      <c r="R50" s="16"/>
-      <c r="S50" s="16"/>
-    </row>
-    <row r="51" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="19"/>
-      <c r="W51" s="19"/>
-      <c r="X51" s="19"/>
-      <c r="Y51" s="19"/>
-      <c r="Z51" s="19"/>
-    </row>
-    <row r="52" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="20"/>
-      <c r="R52" s="20"/>
-      <c r="S52" s="20"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="9"/>
+      <c r="S52" s="9"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G53" s="2"/>
@@ -5370,9 +5547,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corregida la numeración de los entregables
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/Diccionario de la WBS.xlsx
+++ b/Planificación del proyecto/Diccionario de la WBS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Desktop\New folder (2)\Planificación del proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\tpproyect\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="267">
   <si>
     <t>Esta es una versión simplificada para el diccionario de la WBS.</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Productos destacados</t>
-  </si>
-  <si>
-    <t>Proceso mediante el cual se filtrara los productos con el fin de visualizar los mas vendidos y los que cuentan con mayor valoracion</t>
   </si>
   <si>
     <t>Agrupar los productos según la cantidad de ventas y su valoracion</t>
@@ -742,12 +739,6 @@
     <t>1.2.3.2</t>
   </si>
   <si>
-    <t>1.2.3.3</t>
-  </si>
-  <si>
-    <t>1.2.3.4</t>
-  </si>
-  <si>
     <t>1.2.4</t>
   </si>
   <si>
@@ -888,6 +879,12 @@
   <si>
     <t xml:space="preserve">Relacionará cada categoría una de las opciones de la taxonomía de Google de acuerdo a características en común.
 </t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3.3.1.4</t>
   </si>
 </sst>
 </file>
@@ -1460,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1011"/>
+  <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1578,7 +1575,7 @@
         <v>24</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1586,19 +1583,19 @@
         <v>25</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G7" s="32"/>
     </row>
@@ -1607,16 +1604,16 @@
         <v>29</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
@@ -1626,30 +1623,30 @@
         <v>35</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>26</v>
@@ -1664,12 +1661,12 @@
         <v>28</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>30</v>
@@ -1692,7 +1689,7 @@
     </row>
     <row r="12" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>36</v>
@@ -1704,7 +1701,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>38</v>
@@ -1715,34 +1712,34 @@
     </row>
     <row r="13" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>17</v>
@@ -1751,15 +1748,15 @@
         <v>72</v>
       </c>
       <c r="F14" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="15" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>1.2</v>
+      <c r="A15" s="33" t="s">
+        <v>265</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>55</v>
@@ -1774,7 +1771,7 @@
         <v>55</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>57</v>
@@ -1785,130 +1782,130 @@
         <v>45</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F16" s="41"/>
       <c r="G16" s="18" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="31" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="31" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.2">
@@ -1936,7 +1933,7 @@
     </row>
     <row r="23" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>64</v>
@@ -1959,10 +1956,10 @@
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>68</v>
@@ -1980,692 +1977,672 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+    <row r="25" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>199</v>
+      <c r="B26" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>90</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>86</v>
+        <v>220</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="B30" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
+      <c r="E30" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
-        <v>224</v>
-      </c>
       <c r="B31" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="35" t="s">
-        <v>169</v>
+        <v>107</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="31" t="s">
-        <v>100</v>
+      <c r="E31" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="E32" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="36">
+        <v>1.3</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="B34" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>196</v>
+      <c r="C34" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36">
-        <v>1.3</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>40</v>
+      <c r="E34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="16" t="s">
+      <c r="A36" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="12" t="s">
+      <c r="E36" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" s="20" t="s">
+      <c r="E37" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E39" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C40" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>197</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="B41" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D41" s="33" t="s">
+      <c r="D45" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+      <c r="E45" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="F45" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="D42" s="19" t="s">
+      <c r="B47" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="12" t="s">
+      <c r="E47" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D44" s="20" t="s">
+      <c r="E48" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="11" t="s">
+      <c r="E49" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D46" s="18" t="s">
+      <c r="E50" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
+      <c r="Y50" s="8"/>
+      <c r="Z50" s="8"/>
+    </row>
+    <row r="51" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="12">
-        <v>1.4</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="B50" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-      <c r="Q50" s="6"/>
-      <c r="R50" s="6"/>
-      <c r="S50" s="6"/>
-    </row>
-    <row r="51" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="D51" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="F51" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="G51" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
-      <c r="S51" s="7"/>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="8"/>
-      <c r="Y51" s="8"/>
-      <c r="Z51" s="8"/>
-    </row>
-    <row r="52" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C52" s="16" t="s">
+      <c r="E51" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D52" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="16" t="s">
+      <c r="F51" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="G51" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="G52" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
-      <c r="N52" s="9"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9"/>
-      <c r="Q52" s="9"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+    </row>
+    <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G53" s="2"/>
@@ -5540,9 +5517,6 @@
     </row>
     <row r="1010" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1010" s="2"/>
-    </row>
-    <row r="1011" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1011" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Actualizado y adaptado el diccionario con respecto a la WBS v3.0
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/Diccionario de la WBS.xlsx
+++ b/Planificación del proyecto/Diccionario de la WBS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="289">
   <si>
     <t>Esta es una versión simplificada para el diccionario de la WBS.</t>
   </si>
@@ -566,9 +566,6 @@
   </si>
   <si>
     <t>Organización del catalogo</t>
-  </si>
-  <si>
-    <t>Implementar correctamente todas las tareas del usuario, brindando facilidad de utilización de la interfaz y de aprendizaje,y la aceptación de la interfaz por parte del usuario como una herramienta Útil en su trabajo.</t>
   </si>
   <si>
     <t>Slider</t>
@@ -885,6 +882,76 @@
   </si>
   <si>
     <t>1.3.3.1.4</t>
+  </si>
+  <si>
+    <t>Implementar correctamente todas las tareas del usuario, brindando facilidad de utilización de la interfaz y de aprendizaje,y la aceptación de la interfaz por parte del usuario como una herramienta útil en su trabajo.</t>
+  </si>
+  <si>
+    <t>Implementar correctamente todas las tareas del usuario, brindando facilidad de utilización de la interfaz y de aprendizaje,y la aceptación de la interfaz por parte del usuario como una herramienta útil para usar el sistema</t>
+  </si>
+  <si>
+    <t>Que muestre el paso a paso y le otorgue confianza al usuario para ingresar sus datos</t>
+  </si>
+  <si>
+    <t>Información sobre el comercio online de deportes</t>
+  </si>
+  <si>
+    <t>Que le brinda al usuario una expectativa de seriedad del ecommerce en base al trayacto de la empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Que la interfaz permita que el usuario pueda consultar sus dudas y estas sean respondidas en el menor tiempo posible hacia su email</t>
+  </si>
+  <si>
+    <t>Que le dé una buena impresión a los usuarios como elemento principal del home</t>
+  </si>
+  <si>
+    <t>Que se asegure el respaldo de la información de los usuarios</t>
+  </si>
+  <si>
+    <t>Proceso con el fin de brindar al usuario su informacion dentro del e-commerce y donde ademas será capaz de editarla</t>
+  </si>
+  <si>
+    <t>Que los usuarios tengan su información de compras efectuadas con el fin de obtener descuentos</t>
+  </si>
+  <si>
+    <t>Que se pueda renovar la clave</t>
+  </si>
+  <si>
+    <t>Proceso mediante el cual el usuario podrá recuperar la contraseña a partir del mail del usuario</t>
+  </si>
+  <si>
+    <t>Que los usuarios pueden recuperar su clave para no perder el acceso a su cuenta</t>
+  </si>
+  <si>
+    <t>Que la recuperacion de la clave sea segura con el propósito de resguardar los datos del usuario, y se lleve a cabo de la manera más pronta posible</t>
+  </si>
+  <si>
+    <t>Relacionar cada categoría a una de las opciones de la taxonomía de Google de acuerdo a características en común para que las búsquedas sean encontradas más fácilmente</t>
+  </si>
+  <si>
+    <t>Que los productos sean asociados adecuadamente según su categoria, para que Google pueda recomendar dichos productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceso de petición de solicitudes por parte del usuario para contactarse con los administradores del ecommerce
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que el usuario pueda enviar sus dudas a traves de un formulario </t>
+  </si>
+  <si>
+    <t>Que se renderice rápidamente y tenga buena calidad</t>
+  </si>
+  <si>
+    <t>Proceso por el cual se adjuntarán videos (desde una URL) del producto presentado.</t>
+  </si>
+  <si>
+    <t>Que permita una mayor aproximación al producto y esté en buena calidad</t>
+  </si>
+  <si>
+    <t>Capacidad de administrar los elementos del home a traves de las vistas</t>
+  </si>
+  <si>
+    <t>Permitir, de forma fácil, la correcta administracion de los distintos componentes del sitio</t>
   </si>
 </sst>
 </file>
@@ -957,7 +1024,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -972,19 +1039,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FFDBE5F1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFDBE5F1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,7 +1112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1088,61 +1143,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1154,19 +1155,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1175,7 +1167,79 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1459,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1513,427 +1577,443 @@
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
+    <row r="5" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="38" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="G7" s="32"/>
-    </row>
-    <row r="8" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>189</v>
+      <c r="C13" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="G13" s="11"/>
+      <c r="E13" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>240</v>
+      <c r="F15" s="19" t="s">
+        <v>239</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>192</v>
+      <c r="C17" s="13" t="s">
+        <v>274</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="31" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="C18" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B19" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>194</v>
+      <c r="C19" s="13" t="s">
+        <v>277</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="31" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="C20" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B21" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>255</v>
+      <c r="C21" s="14" t="s">
+        <v>254</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="F21" s="31" t="s">
+      <c r="E21" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>215</v>
+      <c r="A23" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>64</v>
@@ -1955,134 +2035,134 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="B25" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="E25" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="D25" s="16" t="s">
+      <c r="B26" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="E26" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="16" t="s">
+      <c r="B27" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="E27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="B28" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="E28" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>220</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
-        <v>221</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="16" t="s">
         <v>168</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="13" t="s">
         <v>99</v>
       </c>
       <c r="F29" s="11" t="s">
@@ -2093,31 +2173,31 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
         <v>222</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
-        <v>223</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>107</v>
@@ -2139,128 +2219,128 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="43">
+        <v>1.3</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D32" s="16" t="s">
+      <c r="B36" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36">
-        <v>1.3</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
+      <c r="E36" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
         <v>225</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
-        <v>226</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="16" t="s">
         <v>118</v>
       </c>
       <c r="D37" s="11" t="s">
@@ -2269,286 +2349,286 @@
       <c r="E37" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="16" t="s">
         <v>120</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="D38" s="19" t="s">
+      <c r="B39" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="F38" s="28" t="s">
+      <c r="E39" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F39" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+      <c r="G39" s="13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="B39" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" s="33" t="s">
+      <c r="B40" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D40" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="F39" s="37" t="s">
+      <c r="E40" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="35" t="s">
         <v>247</v>
       </c>
-      <c r="G39" s="31" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+      <c r="G40" s="23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="19" t="s">
+      <c r="B44" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="F40" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="12" t="s">
+      <c r="E44" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="12" t="s">
+      <c r="E45" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="25">
+        <v>1.4</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="20" t="s">
+      <c r="E46" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="E47" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="18" t="s">
+      <c r="E48" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12">
-        <v>1.4</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="44" t="s">
         <v>156</v>
       </c>
       <c r="H49" s="6"/>
@@ -2565,25 +2645,25 @@
       <c r="S49" s="6"/>
     </row>
     <row r="50" spans="1:26" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="B50" s="36" t="s">
+      <c r="A50" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="B50" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="D50" s="36" t="s">
+      <c r="D50" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="F50" s="36" t="s">
+      <c r="F50" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="G50" s="38" t="s">
+      <c r="G50" s="36" t="s">
         <v>161</v>
       </c>
       <c r="H50" s="7"/>
@@ -2607,25 +2687,25 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="B51" s="16" t="s">
+      <c r="A51" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="G51" s="16" t="s">
+      <c r="G51" s="11" t="s">
         <v>166</v>
       </c>
       <c r="H51" s="9"/>

</xml_diff>